<commit_message>
1d PM - alpha correction
</commit_message>
<xml_diff>
--- a/tests/reports/run_0/report_eeg-alcohol.xlsx
+++ b/tests/reports/run_0/report_eeg-alcohol.xlsx
@@ -32,7 +32,7 @@
     <t>Generated on</t>
   </si>
   <si>
-    <t>2025-01-08 11:54:14</t>
+    <t>2025-01-08 12:51:38</t>
   </si>
   <si>
     <t>Run Number</t>
@@ -59,7 +59,7 @@
     <t>eegalcohol</t>
   </si>
   <si>
-    <t>{'mcar': {'mean': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5197922283008971, 'MAE': 0.4543356516868202, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00040984153747558594, 'optimization': 0, 'imputation': 0.00028395652770996094, 'log_imputation': -8.166689402963497}}, '0.1': {'scores': {'RMSE': 1.0659202645786816, 'MAE': 0.9085417731383956, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00040984153747558594, 'optimization': 0, 'imputation': 0.00022745132446289062, 'log_imputation': -8.388574300870511}}, '0.2': {'scores': {'RMSE': 1.1400385999631493, 'MAE': 0.9394950730289477, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00033783912658691406, 'optimization': 0, 'imputation': 0.00013971328735351562, 'log_imputation': -8.875918182741785}}, '0.4': {'scores': {'RMSE': 1.0333061850175014, 'MAE': 0.817160720129779, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0006093978881835938, 'optimization': 0, 'imputation': 0.0001430511474609375, 'log_imputation': -8.85230831710265}}, '0.6': {'scores': {'RMSE': 1.0938413270459857, 'MAE': 0.8545290213993658, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0013480186462402344, 'optimization': 0, 'imputation': 0.00017070770263671875, 'log_imputation': -8.675557805358151}}, '0.8': {'scores': {'RMSE': 1.07436956341757, 'MAE': 0.8291370178635111, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0029239654541015625, 'optimization': 0, 'imputation': 0.0002067089080810547, 'log_imputation': -8.484198995538256}}}}, 'cdrec': {'bayesian': {'0.05': {'scores': {'RMSE': 0.37483452324301586, 'MAE': 0.3375262694281006, 'MI': 1.0397207708399179, 'CORRELATION': 0.7365655689896633}, 'times': {'contamination': 0.00023937225341796875, 'optimization': 0.6537201404571533, 'imputation': 0.0063037872314453125, 'log_imputation': -5.066604678353174}}, '0.1': {'scores': {'RMSE': 1.3799678230195285, 'MAE': 1.1003322284844623, 'MI': 1.732867951399863, 'CORRELATION': -0.500100644242659}, 'times': {'contamination': 0.0003256797790527344, 'optimization': 0.6537201404571533, 'imputation': 0.006911754608154297, 'log_imputation': -4.974531750403096}}, '0.2': {'scores': {'RMSE': 0.5279485898506157, 'MAE': 0.42431581904234256, 'MI': 1.342409426595628, 'CORRELATION': 0.9071070625126642}, 'times': {'contamination': 0.00028443336486816406, 'optimization': 0.6537201404571533, 'imputation': 0.017868995666503906, 'log_imputation': -4.024688153600394}}, '0.4': {'scores': {'RMSE': 0.6529812630837011, 'MAE': 0.42858056477338186, 'MI': 0.8905639332827393, 'CORRELATION': 0.7722811146383882}, 'times': {'contamination': 0.00045752525329589844, 'optimization': 0.6537201404571533, 'imputation': 0.007945537567138672, 'log_imputation': -4.835144820220228}}, '0.6': {'scores': {'RMSE': 0.6798826891423311, 'MAE': 0.47135122101632737, 'MI': 0.6001676421795947, 'CORRELATION': 0.7742382236368857}, 'times': {'contamination': 0.0024785995483398438, 'optimization': 0.6537201404571533, 'imputation': 0.0069272518157958984, 'log_imputation': -4.972292107809591}}, '0.8': {'scores': {'RMSE': 0.7608485588056992, 'MAE': 0.5479154581689161, 'MI': 0.42721564894947844, 'CORRELATION': 0.7017141157422242}, 'times': {'contamination': 0.00587916374206543, 'optimization': 0.6537201404571533, 'imputation': 0.006249427795410156, 'log_imputation': -5.075265372159409}}}}, 'stmvl': {'bayesian': {'0.05': {'scores': {'RMSE': 0.3251125774837754, 'MAE': 0.26797673641099284, 'MI': 1.0397207708399179, 'CORRELATION': 0.6142581896031455}, 'times': {'contamination': 0.00025272369384765625, 'optimization': 0.3357059955596924, 'imputation': 0.061218976974487305, 'log_imputation': -2.793298056246649}}, '0.1': {'scores': {'RMSE': 0.299492451492057, 'MAE': 0.26432871720074347, 'MI': 1.9061547465398494, 'CORRELATION': 0.967896575643492}, 'times': {'contamination': 0.00018143653869628906, 'optimization': 0.3357059955596924, 'imputation': 0.1323375701904297, 'log_imputation': -2.0223992709232097}}, '0.2': {'scores': {'RMSE': 0.32852543256899075, 'MAE': 0.27202573018354975, 'MI': 1.5996631161656454, 'CORRELATION': 0.9558373872353643}, 'times': {'contamination': 0.00032901763916015625, 'optimization': 0.3357059955596924, 'imputation': 0.06464266777038574, 'log_imputation': -2.7388805944206553}}, '0.4': {'scores': {'RMSE': 0.4508488005700101, 'MAE': 0.34941433537269606, 'MI': 0.8543113555966528, 'CORRELATION': 0.8959297471926679}, 'times': {'contamination': 0.00046896934509277344, 'optimization': 0.3357059955596924, 'imputation': 0.05494332313537598, 'log_imputation': -2.901453113515639}}, '0.6': {'scores': {'RMSE': 18.797539991079297, 'MAE': 7.812583796335101, 'MI': 0.36244773022350796, 'CORRELATION': 0.6210142190959098}, 'times': {'contamination': 0.0008962154388427734, 'optimization': 0.3357059955596924, 'imputation': 0.02575063705444336, 'log_imputation': -3.659295912200037}}, '0.8': {'scores': {'RMSE': 3.1451455567216193, 'MAE': 1.1637520656636082, 'MI': 0.0643204354315137, 'CORRELATION': 0.22737088719870605}, 'times': {'contamination': 0.0013713836669921875, 'optimization': 0.3357059955596924, 'imputation': 0.028316020965576172, 'log_imputation': -3.564327522655997}}}}, 'iim': {'bayesian': {'0.05': {'scores': {'RMSE': 0.2311363556202525, 'MAE': 0.22809317150257158, 'MI': 0.6931471805599452, 'CORRELATION': 0.8754093900930757}, 'times': {'contamination': 0.00015234947204589844, 'optimization': 0.8339252471923828, 'imputation': 0.0036537647247314453, 'log_imputation': -5.611997211514384}}, '0.1': {'scores': {'RMSE': 0.21734571962767568, 'MAE': 0.20142183555276616, 'MI': 1.4941751382893083, 'CORRELATION': 0.9836625389334559}, 'times': {'contamination': 0.0002493858337402344, 'optimization': 0.8339252471923828, 'imputation': 0.005974531173706055, 'log_imputation': -5.120249648894781}}, '0.2': {'scores': {'RMSE': 0.2763681623559098, 'MAE': 0.21205899863451294, 'MI': 1.692828654044598, 'CORRELATION': 0.9663556239228223}, 'times': {'contamination': 0.00022602081298828125, 'optimization': 0.8339252471923828, 'imputation': 0.08778023719787598, 'log_imputation': -2.4329188925398264}}, '0.4': {'scores': {'RMSE': 0.32470532661816204, 'MAE': 0.24836184775095202, 'MI': 1.0631520030142667, 'CORRELATION': 0.9435024215665483}, 'times': {'contamination': 0.0006368160247802734, 'optimization': 0.8339252471923828, 'imputation': 0.5580401420593262, 'log_imputation': -0.5833243800139047}}, '0.6': {'scores': {'RMSE': 0.45693859713260937, 'MAE': 0.3350566242376081, 'MI': 0.836724518636222, 'CORRELATION': 0.9015668975756113}, 'times': {'contamination': 0.0013523101806640625, 'optimization': 0.8339252471923828, 'imputation': 1.4875962734222412, 'log_imputation': 0.397161577971691}}, '0.8': {'scores': {'RMSE': 0.7301676007328138, 'MAE': 0.5391664379693699, 'MI': 0.43198783605819785, 'CORRELATION': 0.7329833767632488}, 'times': {'contamination': 0.0027031898498535156, 'optimization': 0.8339252471923828, 'imputation': 2.8330087661743164, 'log_imputation': 1.0413393151515047}}}}, 'mrnn': {'bayesian': {'0.05': {'scores': {'RMSE': 2.6563684177670233, 'MAE': 2.6289027948372983, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0003285408020019531, 'optimization': 37.21349549293518, 'imputation': 9.313198566436768, 'log_imputation': 2.231432594737839}}, '0.1': {'scores': {'RMSE': 2.045766641879113, 'MAE': 1.7992291555274402, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.000408172607421875, 'optimization': 37.21349549293518, 'imputation': 9.40095329284668, 'log_imputation': 2.2408110982665184}}, '0.2': {'scores': {'RMSE': 1.4866964744519828, 'MAE': 1.2498535799157215, 'MI': 0.397640786553919, 'CORRELATION': -0.08276964804710889}, 'times': {'contamination': 0.00039958953857421875, 'optimization': 37.21349549293518, 'imputation': 9.726991415023804, 'log_imputation': 2.2749046412945217}}, '0.4': {'scores': {'RMSE': 1.2317696108511034, 'MAE': 0.9707474883456586, 'MI': 0.15483371229197251, 'CORRELATION': -0.010527558860360244}, 'times': {'contamination': 0.0005564689636230469, 'optimization': 37.21349549293518, 'imputation': 11.057928085327148, 'log_imputation': 2.4031476444877526}}, '0.6': {'scores': {'RMSE': 1.2430465649730325, 'MAE': 1.0234584506854825, 'MI': 0.1447519034646143, 'CORRELATION': 0.017907899469012542}, 'times': {'contamination': 0.001611948013305664, 'optimization': 37.21349549293518, 'imputation': 7.627377986907959, 'log_imputation': 2.031744141008499}}, '0.8': {'scores': {'RMSE': 1.2027168127539818, 'MAE': 0.97815219871441, 'MI': 0.0614813991074497, 'CORRELATION': 0.035724315549045045}, 'times': {'contamination': 0.0026082992553710938, 'optimization': 37.21349549293518, 'imputation': 10.785835981369019, 'log_imputation': 2.3782337901768487}}}}}}</t>
+    <t>{'mcar': {'mean': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5197922283008971, 'MAE': 0.4543356516868202, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00027060508728027344, 'optimization': 0, 'imputation': 0.0001704692840576172, 'log_imputation': -8.676955429624789}}, '0.1': {'scores': {'RMSE': 1.0659202645786816, 'MAE': 0.9085417731383956, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00019931793212890625, 'optimization': 0, 'imputation': 0.00011801719665527344, 'log_imputation': -9.044680209750107}}, '0.2': {'scores': {'RMSE': 1.1400385999631493, 'MAE': 0.9394950730289477, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00022220611572265625, 'optimization': 0, 'imputation': 9.34600830078125e-05, 'log_imputation': -9.277976132528334}}, '0.4': {'scores': {'RMSE': 1.0333061850175014, 'MAE': 0.817160720129779, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00030231475830078125, 'optimization': 0, 'imputation': 6.556510925292969e-05, 'log_imputation': -9.632466874652225}}, '0.6': {'scores': {'RMSE': 1.0938413270459857, 'MAE': 0.8545290213993658, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0005660057067871094, 'optimization': 0, 'imputation': 6.151199340820312e-05, 'log_imputation': -9.696278387397179}}, '0.8': {'scores': {'RMSE': 1.07436956341757, 'MAE': 0.8291370178635111, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0012047290802001953, 'optimization': 0, 'imputation': 6.29425048828125e-05, 'log_imputation': -9.673288869172481}}}}, 'cdrec': {'bayesian': {'0.05': {'scores': {'RMSE': 0.37483452324301586, 'MAE': 0.3375262694281006, 'MI': 1.0397207708399179, 'CORRELATION': 0.7365655689896633}, 'times': {'contamination': 0.00012755393981933594, 'optimization': 0.5108654499053955, 'imputation': 0.004567623138427734, 'log_imputation': -5.388762310375959}}, '0.1': {'scores': {'RMSE': 1.3799678230195285, 'MAE': 1.1003322284844623, 'MI': 1.732867951399863, 'CORRELATION': -0.500100644242659}, 'times': {'contamination': 0.00033164024353027344, 'optimization': 0.5108654499053955, 'imputation': 0.004395723342895508, 'log_imputation': -5.427123178248406}}, '0.2': {'scores': {'RMSE': 0.5279485898506157, 'MAE': 0.42431581904234256, 'MI': 1.342409426595628, 'CORRELATION': 0.9071070625126642}, 'times': {'contamination': 0.00019049644470214844, 'optimization': 0.5108654499053955, 'imputation': 0.011562585830688477, 'log_imputation': -4.459980752976466}}, '0.4': {'scores': {'RMSE': 0.6529812630837011, 'MAE': 0.42858056477338186, 'MI': 0.8905639332827393, 'CORRELATION': 0.7722811146383882}, 'times': {'contamination': 0.00030994415283203125, 'optimization': 0.5108654499053955, 'imputation': 0.00451207160949707, 'log_imputation': -5.4009988940131475}}, '0.6': {'scores': {'RMSE': 0.6798826891423311, 'MAE': 0.47135122101632737, 'MI': 0.6001676421795947, 'CORRELATION': 0.7742382236368857}, 'times': {'contamination': 0.0005815029144287109, 'optimization': 0.5108654499053955, 'imputation': 0.0029671192169189453, 'log_imputation': -5.820163757517104}}, '0.8': {'scores': {'RMSE': 0.7608485588056992, 'MAE': 0.5479154581689161, 'MI': 0.42721564894947844, 'CORRELATION': 0.7017141157422242}, 'times': {'contamination': 0.0012214183807373047, 'optimization': 0.5108654499053955, 'imputation': 0.004498004913330078, 'log_imputation': -5.404121333108998}}}}, 'stmvl': {'bayesian': {'0.05': {'scores': {'RMSE': 0.3251125774837754, 'MAE': 0.26797673641099284, 'MI': 1.0397207708399179, 'CORRELATION': 0.6142581896031455}, 'times': {'contamination': 0.00016355514526367188, 'optimization': 0.18949556350708008, 'imputation': 0.0333857536315918, 'log_imputation': -3.399626007968974}}, '0.1': {'scores': {'RMSE': 0.299492451492057, 'MAE': 0.26432871720074347, 'MI': 1.9061547465398494, 'CORRELATION': 0.967896575643492}, 'times': {'contamination': 0.00013828277587890625, 'optimization': 0.18949556350708008, 'imputation': 0.034218549728393555, 'log_imputation': -3.374987392234605}}, '0.2': {'scores': {'RMSE': 0.32852543256899075, 'MAE': 0.27202573018354975, 'MI': 1.5996631161656454, 'CORRELATION': 0.9558373872353643}, 'times': {'contamination': 0.00016021728515625, 'optimization': 0.18949556350708008, 'imputation': 0.03754568099975586, 'log_imputation': -3.282196927367169}}, '0.4': {'scores': {'RMSE': 0.4508488005700101, 'MAE': 0.34941433537269606, 'MI': 0.8543113555966528, 'CORRELATION': 0.8959297471926679}, 'times': {'contamination': 0.0002884864807128906, 'optimization': 0.18949556350708008, 'imputation': 0.03878617286682129, 'log_imputation': -3.2496914652794007}}, '0.6': {'scores': {'RMSE': 18.797539991079297, 'MAE': 7.812583796335101, 'MI': 0.36244773022350796, 'CORRELATION': 0.6210142190959098}, 'times': {'contamination': 0.0006196498870849609, 'optimization': 0.18949556350708008, 'imputation': 0.029697656631469727, 'log_imputation': -3.51668713758367}}, '0.8': {'scores': {'RMSE': 3.1451455567216193, 'MAE': 1.1637520656636082, 'MI': 0.0643204354315137, 'CORRELATION': 0.22737088719870605}, 'times': {'contamination': 0.0011970996856689453, 'optimization': 0.18949556350708008, 'imputation': 0.034436941146850586, 'log_imputation': -3.368625420241316}}}}, 'iim': {'bayesian': {'0.05': {'scores': {'RMSE': 0.2311363556202525, 'MAE': 0.22809317150257158, 'MI': 0.6931471805599452, 'CORRELATION': 0.8754093900930757}, 'times': {'contamination': 0.00020766258239746094, 'optimization': 0.8132822513580322, 'imputation': 0.006684064865112305, 'log_imputation': -5.008028963761024}}, '0.1': {'scores': {'RMSE': 0.21734571962767568, 'MAE': 0.20142183555276616, 'MI': 1.4941751382893083, 'CORRELATION': 0.9836625389334559}, 'times': {'contamination': 0.0001220703125, 'optimization': 0.8132822513580322, 'imputation': 0.008673667907714844, 'log_imputation': -4.747463520246684}}, '0.2': {'scores': {'RMSE': 0.2763681623559098, 'MAE': 0.21205899863451294, 'MI': 1.692828654044598, 'CORRELATION': 0.9663556239228223}, 'times': {'contamination': 0.00015807151794433594, 'optimization': 0.8132822513580322, 'imputation': 0.02692556381225586, 'log_imputation': -3.6146791160565725}}, '0.4': {'scores': {'RMSE': 0.32470532661816204, 'MAE': 0.24836184775095202, 'MI': 1.0631520030142667, 'CORRELATION': 0.9435024215665483}, 'times': {'contamination': 0.00028705596923828125, 'optimization': 0.8132822513580322, 'imputation': 0.19279956817626953, 'log_imputation': -1.6461041365578395}}, '0.6': {'scores': {'RMSE': 0.45693859713260937, 'MAE': 0.3350566242376081, 'MI': 0.836724518636222, 'CORRELATION': 0.9015668975756113}, 'times': {'contamination': 0.0006051063537597656, 'optimization': 0.8132822513580322, 'imputation': 0.5096421241760254, 'log_imputation': -0.6740465168845}}, '0.8': {'scores': {'RMSE': 0.7301676007328138, 'MAE': 0.5391664379693699, 'MI': 0.43198783605819785, 'CORRELATION': 0.7329833767632488}, 'times': {'contamination': 0.001192331314086914, 'optimization': 0.8132822513580322, 'imputation': 2.1703436374664307, 'log_imputation': 0.7748855132944805}}}}, 'mrnn': {'bayesian': {'0.05': {'scores': {'RMSE': 1.5534821982949707, 'MAE': 1.5060357479863002, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00022554397583007812, 'optimization': 33.18070316314697, 'imputation': 7.837775945663452, 'log_imputation': 2.0589551137173507}}, '0.1': {'scores': {'RMSE': 1.2542309808619898, 'MAE': 1.077694959981515, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0003402233123779297, 'optimization': 33.18070316314697, 'imputation': 7.026872158050537, 'log_imputation': 1.9497416790817856}}, '0.2': {'scores': {'RMSE': 1.5269073369222408, 'MAE': 1.229707427832888, 'MI': 0.397640786553919, 'CORRELATION': 0.0010088946702063234}, 'times': {'contamination': 0.00017547607421875, 'optimization': 33.18070316314697, 'imputation': 6.481844186782837, 'log_imputation': 1.8690050665999636}}, '0.4': {'scores': {'RMSE': 1.3382262981163862, 'MAE': 1.079772579102801, 'MI': 0.16557034901046197, 'CORRELATION': 0.016391846298721195}, 'times': {'contamination': 0.0003674030303955078, 'optimization': 33.18070316314697, 'imputation': 8.01118803024292, 'log_imputation': 2.080839068464571}}, '0.6': {'scores': {'RMSE': 1.3571781743580735, 'MAE': 1.0989570438570895, 'MI': 0.10967079612419346, 'CORRELATION': -0.015125969685014458}, 'times': {'contamination': 0.0014710426330566406, 'optimization': 33.18070316314697, 'imputation': 9.495571374893188, 'log_imputation': 2.2508255188511095}}, '0.8': {'scores': {'RMSE': 1.1992433951193446, 'MAE': 0.9771615695053146, 'MI': 0.050276623880035565, 'CORRELATION': 0.00024685644553336644}, 'times': {'contamination': 0.0013470649719238281, 'optimization': 33.18070316314697, 'imputation': 8.68370532989502, 'log_imputation': 2.1614483189086586}}}}}}</t>
   </si>
   <si>
     <t>RMSE: Root Mean Square Error - Measures the average magnitude of error.</t>
@@ -194,22 +194,22 @@
     <t>mrnn</t>
   </si>
   <si>
-    <t>2.6563684178</t>
-  </si>
-  <si>
-    <t>2.0457666419</t>
-  </si>
-  <si>
-    <t>1.4866964745</t>
-  </si>
-  <si>
-    <t>1.2317696109</t>
-  </si>
-  <si>
-    <t>1.2430465650</t>
-  </si>
-  <si>
-    <t>1.2027168128</t>
+    <t>1.5534821983</t>
+  </si>
+  <si>
+    <t>1.2542309809</t>
+  </si>
+  <si>
+    <t>1.5269073369</t>
+  </si>
+  <si>
+    <t>1.3382262981</t>
+  </si>
+  <si>
+    <t>1.3571781744</t>
+  </si>
+  <si>
+    <t>1.1992433951</t>
   </si>
   <si>
     <t>MAE: Mean Absolute Error - Measures the average absolute error.</t>
@@ -290,22 +290,22 @@
     <t>0.5391664380</t>
   </si>
   <si>
-    <t>2.6289027948</t>
-  </si>
-  <si>
-    <t>1.7992291555</t>
-  </si>
-  <si>
-    <t>1.2498535799</t>
-  </si>
-  <si>
-    <t>0.9707474883</t>
-  </si>
-  <si>
-    <t>1.0234584507</t>
-  </si>
-  <si>
-    <t>0.9781521987</t>
+    <t>1.5060357480</t>
+  </si>
+  <si>
+    <t>1.0776949600</t>
+  </si>
+  <si>
+    <t>1.2297074278</t>
+  </si>
+  <si>
+    <t>1.0797725791</t>
+  </si>
+  <si>
+    <t>1.0989570439</t>
+  </si>
+  <si>
+    <t>0.9771615695</t>
   </si>
   <si>
     <t>MI: Mutual Information - Indicates dependency between variables.</t>
@@ -371,13 +371,13 @@
     <t>0.3976407866</t>
   </si>
   <si>
-    <t>0.1548337123</t>
-  </si>
-  <si>
-    <t>0.1447519035</t>
-  </si>
-  <si>
-    <t>0.0614813991</t>
+    <t>0.1655703490</t>
+  </si>
+  <si>
+    <t>0.1096707961</t>
+  </si>
+  <si>
+    <t>0.0502766239</t>
   </si>
   <si>
     <t>CORRELATION: Correlation Coefficient - Indicates linear relationship between variables.</t>
@@ -440,16 +440,16 @@
     <t>0.7329833768</t>
   </si>
   <si>
-    <t>-0.0827696480</t>
-  </si>
-  <si>
-    <t>-0.0105275589</t>
-  </si>
-  <si>
-    <t>0.0179078995</t>
-  </si>
-  <si>
-    <t>0.0357243155</t>
+    <t>0.0010088947</t>
+  </si>
+  <si>
+    <t>0.0163918463</t>
+  </si>
+  <si>
+    <t>-0.0151259697</t>
+  </si>
+  <si>
+    <t>0.0002468564</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
2a PM - gaussian and benchmark
</commit_message>
<xml_diff>
--- a/tests/reports/run_0/report_eeg-alcohol.xlsx
+++ b/tests/reports/run_0/report_eeg-alcohol.xlsx
@@ -32,7 +32,7 @@
     <t>Generated on</t>
   </si>
   <si>
-    <t>2025-01-08 12:51:38</t>
+    <t>2025-01-08 12:57:37</t>
   </si>
   <si>
     <t>Run Number</t>
@@ -59,7 +59,7 @@
     <t>eegalcohol</t>
   </si>
   <si>
-    <t>{'mcar': {'mean': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5197922283008971, 'MAE': 0.4543356516868202, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00027060508728027344, 'optimization': 0, 'imputation': 0.0001704692840576172, 'log_imputation': -8.676955429624789}}, '0.1': {'scores': {'RMSE': 1.0659202645786816, 'MAE': 0.9085417731383956, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00019931793212890625, 'optimization': 0, 'imputation': 0.00011801719665527344, 'log_imputation': -9.044680209750107}}, '0.2': {'scores': {'RMSE': 1.1400385999631493, 'MAE': 0.9394950730289477, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00022220611572265625, 'optimization': 0, 'imputation': 9.34600830078125e-05, 'log_imputation': -9.277976132528334}}, '0.4': {'scores': {'RMSE': 1.0333061850175014, 'MAE': 0.817160720129779, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00030231475830078125, 'optimization': 0, 'imputation': 6.556510925292969e-05, 'log_imputation': -9.632466874652225}}, '0.6': {'scores': {'RMSE': 1.0938413270459857, 'MAE': 0.8545290213993658, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0005660057067871094, 'optimization': 0, 'imputation': 6.151199340820312e-05, 'log_imputation': -9.696278387397179}}, '0.8': {'scores': {'RMSE': 1.07436956341757, 'MAE': 0.8291370178635111, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0012047290802001953, 'optimization': 0, 'imputation': 6.29425048828125e-05, 'log_imputation': -9.673288869172481}}}}, 'cdrec': {'bayesian': {'0.05': {'scores': {'RMSE': 0.37483452324301586, 'MAE': 0.3375262694281006, 'MI': 1.0397207708399179, 'CORRELATION': 0.7365655689896633}, 'times': {'contamination': 0.00012755393981933594, 'optimization': 0.5108654499053955, 'imputation': 0.004567623138427734, 'log_imputation': -5.388762310375959}}, '0.1': {'scores': {'RMSE': 1.3799678230195285, 'MAE': 1.1003322284844623, 'MI': 1.732867951399863, 'CORRELATION': -0.500100644242659}, 'times': {'contamination': 0.00033164024353027344, 'optimization': 0.5108654499053955, 'imputation': 0.004395723342895508, 'log_imputation': -5.427123178248406}}, '0.2': {'scores': {'RMSE': 0.5279485898506157, 'MAE': 0.42431581904234256, 'MI': 1.342409426595628, 'CORRELATION': 0.9071070625126642}, 'times': {'contamination': 0.00019049644470214844, 'optimization': 0.5108654499053955, 'imputation': 0.011562585830688477, 'log_imputation': -4.459980752976466}}, '0.4': {'scores': {'RMSE': 0.6529812630837011, 'MAE': 0.42858056477338186, 'MI': 0.8905639332827393, 'CORRELATION': 0.7722811146383882}, 'times': {'contamination': 0.00030994415283203125, 'optimization': 0.5108654499053955, 'imputation': 0.00451207160949707, 'log_imputation': -5.4009988940131475}}, '0.6': {'scores': {'RMSE': 0.6798826891423311, 'MAE': 0.47135122101632737, 'MI': 0.6001676421795947, 'CORRELATION': 0.7742382236368857}, 'times': {'contamination': 0.0005815029144287109, 'optimization': 0.5108654499053955, 'imputation': 0.0029671192169189453, 'log_imputation': -5.820163757517104}}, '0.8': {'scores': {'RMSE': 0.7608485588056992, 'MAE': 0.5479154581689161, 'MI': 0.42721564894947844, 'CORRELATION': 0.7017141157422242}, 'times': {'contamination': 0.0012214183807373047, 'optimization': 0.5108654499053955, 'imputation': 0.004498004913330078, 'log_imputation': -5.404121333108998}}}}, 'stmvl': {'bayesian': {'0.05': {'scores': {'RMSE': 0.3251125774837754, 'MAE': 0.26797673641099284, 'MI': 1.0397207708399179, 'CORRELATION': 0.6142581896031455}, 'times': {'contamination': 0.00016355514526367188, 'optimization': 0.18949556350708008, 'imputation': 0.0333857536315918, 'log_imputation': -3.399626007968974}}, '0.1': {'scores': {'RMSE': 0.299492451492057, 'MAE': 0.26432871720074347, 'MI': 1.9061547465398494, 'CORRELATION': 0.967896575643492}, 'times': {'contamination': 0.00013828277587890625, 'optimization': 0.18949556350708008, 'imputation': 0.034218549728393555, 'log_imputation': -3.374987392234605}}, '0.2': {'scores': {'RMSE': 0.32852543256899075, 'MAE': 0.27202573018354975, 'MI': 1.5996631161656454, 'CORRELATION': 0.9558373872353643}, 'times': {'contamination': 0.00016021728515625, 'optimization': 0.18949556350708008, 'imputation': 0.03754568099975586, 'log_imputation': -3.282196927367169}}, '0.4': {'scores': {'RMSE': 0.4508488005700101, 'MAE': 0.34941433537269606, 'MI': 0.8543113555966528, 'CORRELATION': 0.8959297471926679}, 'times': {'contamination': 0.0002884864807128906, 'optimization': 0.18949556350708008, 'imputation': 0.03878617286682129, 'log_imputation': -3.2496914652794007}}, '0.6': {'scores': {'RMSE': 18.797539991079297, 'MAE': 7.812583796335101, 'MI': 0.36244773022350796, 'CORRELATION': 0.6210142190959098}, 'times': {'contamination': 0.0006196498870849609, 'optimization': 0.18949556350708008, 'imputation': 0.029697656631469727, 'log_imputation': -3.51668713758367}}, '0.8': {'scores': {'RMSE': 3.1451455567216193, 'MAE': 1.1637520656636082, 'MI': 0.0643204354315137, 'CORRELATION': 0.22737088719870605}, 'times': {'contamination': 0.0011970996856689453, 'optimization': 0.18949556350708008, 'imputation': 0.034436941146850586, 'log_imputation': -3.368625420241316}}}}, 'iim': {'bayesian': {'0.05': {'scores': {'RMSE': 0.2311363556202525, 'MAE': 0.22809317150257158, 'MI': 0.6931471805599452, 'CORRELATION': 0.8754093900930757}, 'times': {'contamination': 0.00020766258239746094, 'optimization': 0.8132822513580322, 'imputation': 0.006684064865112305, 'log_imputation': -5.008028963761024}}, '0.1': {'scores': {'RMSE': 0.21734571962767568, 'MAE': 0.20142183555276616, 'MI': 1.4941751382893083, 'CORRELATION': 0.9836625389334559}, 'times': {'contamination': 0.0001220703125, 'optimization': 0.8132822513580322, 'imputation': 0.008673667907714844, 'log_imputation': -4.747463520246684}}, '0.2': {'scores': {'RMSE': 0.2763681623559098, 'MAE': 0.21205899863451294, 'MI': 1.692828654044598, 'CORRELATION': 0.9663556239228223}, 'times': {'contamination': 0.00015807151794433594, 'optimization': 0.8132822513580322, 'imputation': 0.02692556381225586, 'log_imputation': -3.6146791160565725}}, '0.4': {'scores': {'RMSE': 0.32470532661816204, 'MAE': 0.24836184775095202, 'MI': 1.0631520030142667, 'CORRELATION': 0.9435024215665483}, 'times': {'contamination': 0.00028705596923828125, 'optimization': 0.8132822513580322, 'imputation': 0.19279956817626953, 'log_imputation': -1.6461041365578395}}, '0.6': {'scores': {'RMSE': 0.45693859713260937, 'MAE': 0.3350566242376081, 'MI': 0.836724518636222, 'CORRELATION': 0.9015668975756113}, 'times': {'contamination': 0.0006051063537597656, 'optimization': 0.8132822513580322, 'imputation': 0.5096421241760254, 'log_imputation': -0.6740465168845}}, '0.8': {'scores': {'RMSE': 0.7301676007328138, 'MAE': 0.5391664379693699, 'MI': 0.43198783605819785, 'CORRELATION': 0.7329833767632488}, 'times': {'contamination': 0.001192331314086914, 'optimization': 0.8132822513580322, 'imputation': 2.1703436374664307, 'log_imputation': 0.7748855132944805}}}}, 'mrnn': {'bayesian': {'0.05': {'scores': {'RMSE': 1.5534821982949707, 'MAE': 1.5060357479863002, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00022554397583007812, 'optimization': 33.18070316314697, 'imputation': 7.837775945663452, 'log_imputation': 2.0589551137173507}}, '0.1': {'scores': {'RMSE': 1.2542309808619898, 'MAE': 1.077694959981515, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0003402233123779297, 'optimization': 33.18070316314697, 'imputation': 7.026872158050537, 'log_imputation': 1.9497416790817856}}, '0.2': {'scores': {'RMSE': 1.5269073369222408, 'MAE': 1.229707427832888, 'MI': 0.397640786553919, 'CORRELATION': 0.0010088946702063234}, 'times': {'contamination': 0.00017547607421875, 'optimization': 33.18070316314697, 'imputation': 6.481844186782837, 'log_imputation': 1.8690050665999636}}, '0.4': {'scores': {'RMSE': 1.3382262981163862, 'MAE': 1.079772579102801, 'MI': 0.16557034901046197, 'CORRELATION': 0.016391846298721195}, 'times': {'contamination': 0.0003674030303955078, 'optimization': 33.18070316314697, 'imputation': 8.01118803024292, 'log_imputation': 2.080839068464571}}, '0.6': {'scores': {'RMSE': 1.3571781743580735, 'MAE': 1.0989570438570895, 'MI': 0.10967079612419346, 'CORRELATION': -0.015125969685014458}, 'times': {'contamination': 0.0014710426330566406, 'optimization': 33.18070316314697, 'imputation': 9.495571374893188, 'log_imputation': 2.2508255188511095}}, '0.8': {'scores': {'RMSE': 1.1992433951193446, 'MAE': 0.9771615695053146, 'MI': 0.050276623880035565, 'CORRELATION': 0.00024685644553336644}, 'times': {'contamination': 0.0013470649719238281, 'optimization': 33.18070316314697, 'imputation': 8.68370532989502, 'log_imputation': 2.1614483189086586}}}}}}</t>
+    <t>{'mcar': {'mean': {'bayesian': {'0.05': {'scores': {'RMSE': 0.5197922283008971, 'MAE': 0.4543356516868202, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0004885196685791016, 'optimization': 0, 'imputation': 0.0002512931823730469, 'log_imputation': -8.28889024321749}}, '0.1': {'scores': {'RMSE': 1.0659202645786816, 'MAE': 0.9085417731383956, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0003097057342529297, 'optimization': 0, 'imputation': 0.00014352798461914062, 'log_imputation': -8.848980527009976}}, '0.2': {'scores': {'RMSE': 1.1400385999631493, 'MAE': 0.9394950730289477, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00023746490478515625, 'optimization': 0, 'imputation': 9.608268737792969e-05, 'log_imputation': -9.250301410372114}}, '0.4': {'scores': {'RMSE': 1.0333061850175014, 'MAE': 0.817160720129779, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00040912628173828125, 'optimization': 0, 'imputation': 7.462501525878906e-05, 'log_imputation': -9.503034781778643}}, '0.6': {'scores': {'RMSE': 1.0938413270459857, 'MAE': 0.8545290213993658, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0006306171417236328, 'optimization': 0, 'imputation': 9.202957153320312e-05, 'log_imputation': -9.293400602853966}}, '0.8': {'scores': {'RMSE': 1.07436956341757, 'MAE': 0.8291370178635111, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.001354217529296875, 'optimization': 0, 'imputation': 6.961822509765625e-05, 'log_imputation': -9.572484170050515}}}}, 'cdrec': {'bayesian': {'0.05': {'scores': {'RMSE': 0.37483452324301586, 'MAE': 0.3375262694281006, 'MI': 1.0397207708399179, 'CORRELATION': 0.7365655689896633}, 'times': {'contamination': 0.00011134147644042969, 'optimization': 0.5079936981201172, 'imputation': 0.004687070846557617, 'log_imputation': -5.362947444611191}}, '0.1': {'scores': {'RMSE': 1.3799678230195285, 'MAE': 1.1003322284844623, 'MI': 1.732867951399863, 'CORRELATION': -0.500100644242659}, 'times': {'contamination': 0.0003001689910888672, 'optimization': 0.5079936981201172, 'imputation': 0.0036382675170898438, 'log_imputation': -5.616247667480349}}, '0.2': {'scores': {'RMSE': 0.5279485898506157, 'MAE': 0.42431581904234256, 'MI': 1.342409426595628, 'CORRELATION': 0.9071070625126642}, 'times': {'contamination': 0.00042891502380371094, 'optimization': 0.5079936981201172, 'imputation': 0.015071868896484375, 'log_imputation': -4.194925259667625}}, '0.4': {'scores': {'RMSE': 0.6529812630837011, 'MAE': 0.42858056477338186, 'MI': 0.8905639332827393, 'CORRELATION': 0.7722811146383882}, 'times': {'contamination': 0.00032210350036621094, 'optimization': 0.5079936981201172, 'imputation': 0.008674860000610352, 'log_imputation': -4.74732609153761}}, '0.6': {'scores': {'RMSE': 0.6798826891423311, 'MAE': 0.47135122101632737, 'MI': 0.6001676421795947, 'CORRELATION': 0.7742382236368857}, 'times': {'contamination': 0.0015621185302734375, 'optimization': 0.5079936981201172, 'imputation': 0.009982585906982422, 'log_imputation': -4.606913113305608}}, '0.8': {'scores': {'RMSE': 0.7608485588056992, 'MAE': 0.5479154581689161, 'MI': 0.42721564894947844, 'CORRELATION': 0.7017141157422242}, 'times': {'contamination': 0.003453493118286133, 'optimization': 0.5079936981201172, 'imputation': 0.0073740482330322266, 'log_imputation': -4.9097884382325}}}}, 'stmvl': {'bayesian': {'0.05': {'scores': {'RMSE': 0.3251125774837754, 'MAE': 0.26797673641099284, 'MI': 1.0397207708399179, 'CORRELATION': 0.6142581896031455}, 'times': {'contamination': 0.00034546852111816406, 'optimization': 0.23014473915100098, 'imputation': 0.06188774108886719, 'log_imputation': -2.7824331627034407}}, '0.1': {'scores': {'RMSE': 0.299492451492057, 'MAE': 0.26432871720074347, 'MI': 1.9061547465398494, 'CORRELATION': 0.967896575643492}, 'times': {'contamination': 0.0001323223114013672, 'optimization': 0.23014473915100098, 'imputation': 0.049030303955078125, 'log_imputation': -3.015316723968884}}, '0.2': {'scores': {'RMSE': 0.32852543256899075, 'MAE': 0.27202573018354975, 'MI': 1.5996631161656454, 'CORRELATION': 0.9558373872353643}, 'times': {'contamination': 0.00020933151245117188, 'optimization': 0.23014473915100098, 'imputation': 0.04225325584411621, 'log_imputation': -3.164073866748831}}, '0.4': {'scores': {'RMSE': 0.4508488005700101, 'MAE': 0.34941433537269606, 'MI': 0.8543113555966528, 'CORRELATION': 0.8959297471926679}, 'times': {'contamination': 0.0003197193145751953, 'optimization': 0.23014473915100098, 'imputation': 0.046411752700805664, 'log_imputation': -3.070202560857029}}, '0.6': {'scores': {'RMSE': 18.797539991079297, 'MAE': 7.812583796335101, 'MI': 0.36244773022350796, 'CORRELATION': 0.6210142190959098}, 'times': {'contamination': 0.0006625652313232422, 'optimization': 0.23014473915100098, 'imputation': 0.043074607849121094, 'log_imputation': -3.144821600518555}}, '0.8': {'scores': {'RMSE': 3.1451455567216193, 'MAE': 1.1637520656636082, 'MI': 0.0643204354315137, 'CORRELATION': 0.22737088719870605}, 'times': {'contamination': 0.0013301372528076172, 'optimization': 0.23014473915100098, 'imputation': 0.03976869583129883, 'log_imputation': -3.2246752130762237}}}}, 'iim': {'bayesian': {'0.05': {'scores': {'RMSE': 0.2311363556202525, 'MAE': 0.22809317150257158, 'MI': 0.6931471805599452, 'CORRELATION': 0.8754093900930757}, 'times': {'contamination': 0.00014829635620117188, 'optimization': 0.8548746109008789, 'imputation': 0.006244659423828125, 'log_imputation': -5.0760286727078805}}, '0.1': {'scores': {'RMSE': 0.21734571962767568, 'MAE': 0.20142183555276616, 'MI': 1.4941751382893083, 'CORRELATION': 0.9836625389334559}, 'times': {'contamination': 0.000431060791015625, 'optimization': 0.8548746109008789, 'imputation': 0.016748428344726562, 'log_imputation': -4.089450855278965}}, '0.2': {'scores': {'RMSE': 0.2763681623559098, 'MAE': 0.21205899863451294, 'MI': 1.692828654044598, 'CORRELATION': 0.9663556239228223}, 'times': {'contamination': 0.0001976490020751953, 'optimization': 0.8548746109008789, 'imputation': 0.038770198822021484, 'log_imputation': -3.2501033990684074}}, '0.4': {'scores': {'RMSE': 0.32470532661816204, 'MAE': 0.24836184775095202, 'MI': 1.0631520030142667, 'CORRELATION': 0.9435024215665483}, 'times': {'contamination': 0.0003495216369628906, 'optimization': 0.8548746109008789, 'imputation': 0.21004080772399902, 'log_imputation': -1.5604534446476055}}, '0.6': {'scores': {'RMSE': 0.45693859713260937, 'MAE': 0.3350566242376081, 'MI': 0.836724518636222, 'CORRELATION': 0.9015668975756113}, 'times': {'contamination': 0.0006783008575439453, 'optimization': 0.8548746109008789, 'imputation': 0.6758015155792236, 'log_imputation': -0.39185586205985784}}, '0.8': {'scores': {'RMSE': 0.7301676007328138, 'MAE': 0.5391664379693699, 'MI': 0.43198783605819785, 'CORRELATION': 0.7329833767632488}, 'times': {'contamination': 0.0021584033966064453, 'optimization': 0.8548746109008789, 'imputation': 3.9872961044311523, 'log_imputation': 1.383113333118614}}}}, 'mrnn': {'bayesian': {'0.05': {'scores': {'RMSE': 1.7800071295936744, 'MAE': 1.7387530345617206, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.0002582073211669922, 'optimization': 29.687320470809937, 'imputation': 6.463064670562744, 'log_imputation': 1.866103612506844}}, '0.1': {'scores': {'RMSE': 1.4143718875049651, 'MAE': 1.2042932544309777, 'MI': 0.0, 'CORRELATION': 0}, 'times': {'contamination': 0.00035381317138671875, 'optimization': 29.687320470809937, 'imputation': 6.938860893249512, 'log_imputation': 1.937137624627478}}, '0.2': {'scores': {'RMSE': 1.468628957888676, 'MAE': 1.177928404642071, 'MI': 0.2888172042752689, 'CORRELATION': 0.27089827066191574}, 'times': {'contamination': 0.0003085136413574219, 'optimization': 29.687320470809937, 'imputation': 7.3980393409729, 'log_imputation': 2.0012150111810514}}, '0.4': {'scores': {'RMSE': 1.2420980860848794, 'MAE': 0.9793021593310115, 'MI': 0.16817610173038405, 'CORRELATION': 0.06862278658494796}, 'times': {'contamination': 0.0005781650543212891, 'optimization': 29.687320470809937, 'imputation': 7.899038076400757, 'log_imputation': 2.066740989578406}}, '0.6': {'scores': {'RMSE': 1.3361811680109383, 'MAE': 1.0908161906800318, 'MI': 0.1307724816846375, 'CORRELATION': 0.07966669775362903}, 'times': {'contamination': 0.0015287399291992188, 'optimization': 29.687320470809937, 'imputation': 5.665785551071167, 'log_imputation': 1.7344455523106883}}, '0.8': {'scores': {'RMSE': 1.2352164167350344, 'MAE': 0.9969833725134342, 'MI': 0.08739712471151846, 'CORRELATION': 0.03209263198570942}, 'times': {'contamination': 0.0018906593322753906, 'optimization': 29.687320470809937, 'imputation': 7.642791986465454, 'log_imputation': 2.0337629796749472}}}}}}</t>
   </si>
   <si>
     <t>RMSE: Root Mean Square Error - Measures the average magnitude of error.</t>
@@ -194,22 +194,22 @@
     <t>mrnn</t>
   </si>
   <si>
-    <t>1.5534821983</t>
-  </si>
-  <si>
-    <t>1.2542309809</t>
-  </si>
-  <si>
-    <t>1.5269073369</t>
-  </si>
-  <si>
-    <t>1.3382262981</t>
-  </si>
-  <si>
-    <t>1.3571781744</t>
-  </si>
-  <si>
-    <t>1.1992433951</t>
+    <t>1.7800071296</t>
+  </si>
+  <si>
+    <t>1.4143718875</t>
+  </si>
+  <si>
+    <t>1.4686289579</t>
+  </si>
+  <si>
+    <t>1.2420980861</t>
+  </si>
+  <si>
+    <t>1.3361811680</t>
+  </si>
+  <si>
+    <t>1.2352164167</t>
   </si>
   <si>
     <t>MAE: Mean Absolute Error - Measures the average absolute error.</t>
@@ -290,22 +290,22 @@
     <t>0.5391664380</t>
   </si>
   <si>
-    <t>1.5060357480</t>
-  </si>
-  <si>
-    <t>1.0776949600</t>
-  </si>
-  <si>
-    <t>1.2297074278</t>
-  </si>
-  <si>
-    <t>1.0797725791</t>
-  </si>
-  <si>
-    <t>1.0989570439</t>
-  </si>
-  <si>
-    <t>0.9771615695</t>
+    <t>1.7387530346</t>
+  </si>
+  <si>
+    <t>1.2042932544</t>
+  </si>
+  <si>
+    <t>1.1779284046</t>
+  </si>
+  <si>
+    <t>0.9793021593</t>
+  </si>
+  <si>
+    <t>1.0908161907</t>
+  </si>
+  <si>
+    <t>0.9969833725</t>
   </si>
   <si>
     <t>MI: Mutual Information - Indicates dependency between variables.</t>
@@ -368,16 +368,16 @@
     <t>0.4319878361</t>
   </si>
   <si>
-    <t>0.3976407866</t>
-  </si>
-  <si>
-    <t>0.1655703490</t>
-  </si>
-  <si>
-    <t>0.1096707961</t>
-  </si>
-  <si>
-    <t>0.0502766239</t>
+    <t>0.2888172043</t>
+  </si>
+  <si>
+    <t>0.1681761017</t>
+  </si>
+  <si>
+    <t>0.1307724817</t>
+  </si>
+  <si>
+    <t>0.0873971247</t>
   </si>
   <si>
     <t>CORRELATION: Correlation Coefficient - Indicates linear relationship between variables.</t>
@@ -440,16 +440,16 @@
     <t>0.7329833768</t>
   </si>
   <si>
-    <t>0.0010088947</t>
-  </si>
-  <si>
-    <t>0.0163918463</t>
-  </si>
-  <si>
-    <t>-0.0151259697</t>
-  </si>
-  <si>
-    <t>0.0002468564</t>
+    <t>0.2708982707</t>
+  </si>
+  <si>
+    <t>0.0686227866</t>
+  </si>
+  <si>
+    <t>0.0796666978</t>
+  </si>
+  <si>
+    <t>0.0320926320</t>
   </si>
 </sst>
 </file>

</xml_diff>